<commit_message>
Daily tasks solving (additional)
</commit_message>
<xml_diff>
--- a/Interview preparation 2019-2020.xlsx
+++ b/Interview preparation 2019-2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\LeetCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A1B97A-E5C5-4DA6-A103-F633EA082476}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2AC157-5C76-49EA-9902-29E38D2F4CEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5850" yWindow="4620" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6108" yWindow="588" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="316">
   <si>
     <t>Number</t>
   </si>
@@ -967,6 +967,9 @@
   </si>
   <si>
     <t>Arranging Coins</t>
+  </si>
+  <si>
+    <t>Heaters</t>
   </si>
 </sst>
 </file>
@@ -976,12 +979,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1210,7 +1221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1219,20 +1230,21 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1247,7 +1259,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1283,7 +1295,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6C50ED8C-B740-45AF-BDA6-0857A5A322F4}" name="Таблица1" displayName="Таблица1" ref="A1:G1048576" totalsRowShown="0">
   <autoFilter ref="A1:G1048576" xr:uid="{059DB994-AB16-4545-BFB1-8470F05D6AA7}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G256">
+  <sortState ref="A2:G256">
     <sortCondition ref="G1:G1048576"/>
   </sortState>
   <tableColumns count="7">
@@ -1300,9 +1312,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1340,7 +1352,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1446,7 +1458,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1597,24 +1609,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:G281"/>
+  <dimension ref="A1:G282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A272" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B283" sqref="B283"/>
+    <sheetView tabSelected="1" topLeftCell="A268" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F283" sqref="F283"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="66.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="66.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1637,7 +1649,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>509</v>
       </c>
@@ -1660,7 +1672,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>766</v>
       </c>
@@ -1683,7 +1695,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>832</v>
       </c>
@@ -1706,7 +1718,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>867</v>
       </c>
@@ -1729,7 +1741,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>905</v>
       </c>
@@ -1752,7 +1764,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>922</v>
       </c>
@@ -1775,7 +1787,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>985</v>
       </c>
@@ -1798,7 +1810,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>999</v>
       </c>
@@ -1821,7 +1833,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>1051</v>
       </c>
@@ -1844,7 +1856,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>238</v>
       </c>
@@ -1867,7 +1879,7 @@
         <v>43643</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>442</v>
       </c>
@@ -1890,7 +1902,7 @@
         <v>43643</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>950</v>
       </c>
@@ -1913,7 +1925,7 @@
         <v>43643</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>41</v>
       </c>
@@ -1936,7 +1948,7 @@
         <v>43644</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>57</v>
       </c>
@@ -1959,7 +1971,7 @@
         <v>43644</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>768</v>
       </c>
@@ -1982,7 +1994,7 @@
         <v>43644</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>769</v>
       </c>
@@ -2005,7 +2017,7 @@
         <v>43644</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>728</v>
       </c>
@@ -2028,7 +2040,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>812</v>
       </c>
@@ -2051,7 +2063,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>868</v>
       </c>
@@ -2074,7 +2086,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>883</v>
       </c>
@@ -2097,7 +2109,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>908</v>
       </c>
@@ -2120,7 +2132,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>942</v>
       </c>
@@ -2143,7 +2155,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1009</v>
       </c>
@@ -2166,7 +2178,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1103</v>
       </c>
@@ -2189,7 +2201,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>789</v>
       </c>
@@ -2212,7 +2224,7 @@
         <v>43648</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>885</v>
       </c>
@@ -2235,7 +2247,7 @@
         <v>43648</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1006</v>
       </c>
@@ -2258,7 +2270,7 @@
         <v>43648</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1017</v>
       </c>
@@ -2281,7 +2293,7 @@
         <v>43648</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>335</v>
       </c>
@@ -2304,7 +2316,7 @@
         <v>43649</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>233</v>
       </c>
@@ -2327,7 +2339,7 @@
         <v>43651</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>780</v>
       </c>
@@ -2350,7 +2362,7 @@
         <v>43651</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>744</v>
       </c>
@@ -2373,7 +2385,7 @@
         <v>43652</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2396,7 +2408,7 @@
         <v>43657</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>719</v>
       </c>
@@ -2419,7 +2431,7 @@
         <v>43657</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>657</v>
       </c>
@@ -2442,7 +2454,7 @@
         <v>43658</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>709</v>
       </c>
@@ -2465,7 +2477,7 @@
         <v>43658</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>804</v>
       </c>
@@ -2488,7 +2500,7 @@
         <v>43658</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>929</v>
       </c>
@@ -2511,7 +2523,7 @@
         <v>43658</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1108</v>
       </c>
@@ -2534,7 +2546,7 @@
         <v>43658</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>521</v>
       </c>
@@ -2557,7 +2569,7 @@
         <v>43659</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>824</v>
       </c>
@@ -2580,7 +2592,7 @@
         <v>43659</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>893</v>
       </c>
@@ -2603,7 +2615,7 @@
         <v>43659</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>917</v>
       </c>
@@ -2626,7 +2638,7 @@
         <v>43659</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>937</v>
       </c>
@@ -2649,7 +2661,7 @@
         <v>43659</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>890</v>
       </c>
@@ -2672,7 +2684,7 @@
         <v>43661</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>537</v>
       </c>
@@ -2695,7 +2707,7 @@
         <v>43662</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>791</v>
       </c>
@@ -2718,7 +2730,7 @@
         <v>43662</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1016</v>
       </c>
@@ -2741,7 +2753,7 @@
         <v>43662</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1106</v>
       </c>
@@ -2764,7 +2776,7 @@
         <v>43663</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>461</v>
       </c>
@@ -2787,7 +2799,7 @@
         <v>43667</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>476</v>
       </c>
@@ -2810,7 +2822,7 @@
         <v>43668</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>762</v>
       </c>
@@ -2833,7 +2845,7 @@
         <v>43668</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>136</v>
       </c>
@@ -2856,7 +2868,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>190</v>
       </c>
@@ -2879,7 +2891,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>191</v>
       </c>
@@ -2902,7 +2914,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>231</v>
       </c>
@@ -2925,7 +2937,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>268</v>
       </c>
@@ -2948,7 +2960,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>342</v>
       </c>
@@ -2971,7 +2983,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>371</v>
       </c>
@@ -2994,7 +3006,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>389</v>
       </c>
@@ -3017,7 +3029,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>405</v>
       </c>
@@ -3040,7 +3052,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>260</v>
       </c>
@@ -3063,7 +3075,7 @@
         <v>43670</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>137</v>
       </c>
@@ -3086,7 +3098,7 @@
         <v>43671</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>201</v>
       </c>
@@ -3109,7 +3121,7 @@
         <v>43671</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>318</v>
       </c>
@@ -3132,7 +3144,7 @@
         <v>43671</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>477</v>
       </c>
@@ -3155,7 +3167,7 @@
         <v>43671</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>187</v>
       </c>
@@ -3178,7 +3190,7 @@
         <v>43672</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>88</v>
       </c>
@@ -3201,7 +3213,7 @@
         <v>43675</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>125</v>
       </c>
@@ -3224,7 +3236,7 @@
         <v>43675</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>345</v>
       </c>
@@ -3247,7 +3259,7 @@
         <v>43675</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>844</v>
       </c>
@@ -3270,7 +3282,7 @@
         <v>43675</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>925</v>
       </c>
@@ -3293,7 +3305,7 @@
         <v>43675</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>977</v>
       </c>
@@ -3316,7 +3328,7 @@
         <v>43675</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>532</v>
       </c>
@@ -3339,7 +3351,7 @@
         <v>43676</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>11</v>
       </c>
@@ -3362,7 +3374,7 @@
         <v>43677</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>16</v>
       </c>
@@ -3385,7 +3397,7 @@
         <v>43677</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>986</v>
       </c>
@@ -3408,7 +3420,7 @@
         <v>43677</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>75</v>
       </c>
@@ -3431,7 +3443,7 @@
         <v>43678</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>80</v>
       </c>
@@ -3454,7 +3466,7 @@
         <v>43678</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A81" s="8">
         <v>904</v>
       </c>
@@ -3477,7 +3489,7 @@
         <v>43678</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>21</v>
       </c>
@@ -3500,7 +3512,7 @@
         <v>43682</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>237</v>
       </c>
@@ -3523,7 +3535,7 @@
         <v>43682</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>876</v>
       </c>
@@ -3546,7 +3558,7 @@
         <v>43682</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3569,7 +3581,7 @@
         <v>43683</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>203</v>
       </c>
@@ -3592,7 +3604,7 @@
         <v>43683</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>234</v>
       </c>
@@ -3615,7 +3627,7 @@
         <v>43683</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>1019</v>
       </c>
@@ -3638,7 +3650,7 @@
         <v>43684</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2</v>
       </c>
@@ -3661,7 +3673,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>328</v>
       </c>
@@ -3684,7 +3696,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>445</v>
       </c>
@@ -3707,7 +3719,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>206</v>
       </c>
@@ -3730,7 +3742,7 @@
         <v>43687</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>725</v>
       </c>
@@ -3753,7 +3765,7 @@
         <v>43687</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>25</v>
       </c>
@@ -3776,7 +3788,7 @@
         <v>43689</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>92</v>
       </c>
@@ -3799,7 +3811,7 @@
         <v>43689</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>641</v>
       </c>
@@ -3822,7 +3834,7 @@
         <v>43690</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>622</v>
       </c>
@@ -3845,7 +3857,7 @@
         <v>43691</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>469</v>
       </c>
@@ -3868,7 +3880,7 @@
         <v>43692</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>682</v>
       </c>
@@ -3891,7 +3903,7 @@
         <v>43692</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>862</v>
       </c>
@@ -3914,7 +3926,7 @@
         <v>43692</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>1047</v>
       </c>
@@ -3937,7 +3949,7 @@
         <v>43692</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>232</v>
       </c>
@@ -3960,7 +3972,7 @@
         <v>43693</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>1021</v>
       </c>
@@ -3983,7 +3995,7 @@
         <v>43693</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>20</v>
       </c>
@@ -4006,7 +4018,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>155</v>
       </c>
@@ -4029,7 +4041,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>225</v>
       </c>
@@ -4052,7 +4064,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>946</v>
       </c>
@@ -4075,7 +4087,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>503</v>
       </c>
@@ -4098,7 +4110,7 @@
         <v>43697</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>895</v>
       </c>
@@ -4121,7 +4133,7 @@
         <v>43698</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>50</v>
       </c>
@@ -4144,7 +4156,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>70</v>
       </c>
@@ -4167,7 +4179,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>95</v>
       </c>
@@ -4190,7 +4202,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>104</v>
       </c>
@@ -4213,7 +4225,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>118</v>
       </c>
@@ -4236,7 +4248,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>119</v>
       </c>
@@ -4259,7 +4271,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>775</v>
       </c>
@@ -4282,7 +4294,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>912</v>
       </c>
@@ -4305,7 +4317,7 @@
         <v>43707</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>98</v>
       </c>
@@ -4328,7 +4340,7 @@
         <v>43709</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>240</v>
       </c>
@@ -4351,7 +4363,7 @@
         <v>43710</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>37</v>
       </c>
@@ -4374,7 +4386,7 @@
         <v>43713</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>51</v>
       </c>
@@ -4397,7 +4409,7 @@
         <v>43713</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>52</v>
       </c>
@@ -4420,7 +4432,7 @@
         <v>43713</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>17</v>
       </c>
@@ -4443,7 +4455,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>22</v>
       </c>
@@ -4466,7 +4478,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>46</v>
       </c>
@@ -4489,7 +4501,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>77</v>
       </c>
@@ -4512,7 +4524,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>100</v>
       </c>
@@ -4535,7 +4547,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>401</v>
       </c>
@@ -4558,7 +4570,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>784</v>
       </c>
@@ -4581,7 +4593,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>39</v>
       </c>
@@ -4604,7 +4616,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>40</v>
       </c>
@@ -4627,7 +4639,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>216</v>
       </c>
@@ -4650,7 +4662,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>1</v>
       </c>
@@ -4673,7 +4685,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>217</v>
       </c>
@@ -4696,7 +4708,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>219</v>
       </c>
@@ -4719,7 +4731,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>349</v>
       </c>
@@ -4742,7 +4754,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>705</v>
       </c>
@@ -4765,7 +4777,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>706</v>
       </c>
@@ -4788,7 +4800,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>36</v>
       </c>
@@ -4811,7 +4823,7 @@
         <v>43720</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>49</v>
       </c>
@@ -4834,7 +4846,7 @@
         <v>43720</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>205</v>
       </c>
@@ -4857,7 +4869,7 @@
         <v>43720</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>387</v>
       </c>
@@ -4880,7 +4892,7 @@
         <v>43720</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>599</v>
       </c>
@@ -4903,7 +4915,7 @@
         <v>43720</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>3</v>
       </c>
@@ -4926,7 +4938,7 @@
         <v>43721</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>347</v>
       </c>
@@ -4949,7 +4961,7 @@
         <v>43721</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>380</v>
       </c>
@@ -4972,7 +4984,7 @@
         <v>43721</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>454</v>
       </c>
@@ -4995,7 +5007,7 @@
         <v>43721</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>652</v>
       </c>
@@ -5018,7 +5030,7 @@
         <v>43721</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>771</v>
       </c>
@@ -5041,7 +5053,7 @@
         <v>43721</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>144</v>
       </c>
@@ -5064,7 +5076,7 @@
         <v>43724</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>94</v>
       </c>
@@ -5087,7 +5099,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>102</v>
       </c>
@@ -5110,7 +5122,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>145</v>
       </c>
@@ -5133,7 +5145,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>101</v>
       </c>
@@ -5156,7 +5168,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>105</v>
       </c>
@@ -5179,7 +5191,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>106</v>
       </c>
@@ -5202,7 +5214,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>116</v>
       </c>
@@ -5225,7 +5237,7 @@
         <v>43727</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>117</v>
       </c>
@@ -5248,7 +5260,7 @@
         <v>43727</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>236</v>
       </c>
@@ -5271,7 +5283,7 @@
         <v>43727</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>297</v>
       </c>
@@ -5294,7 +5306,7 @@
         <v>43727</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>429</v>
       </c>
@@ -5317,7 +5329,7 @@
         <v>43731</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>559</v>
       </c>
@@ -5340,7 +5352,7 @@
         <v>43731</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>589</v>
       </c>
@@ -5363,7 +5375,7 @@
         <v>43731</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>590</v>
       </c>
@@ -5386,7 +5398,7 @@
         <v>43731</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>173</v>
       </c>
@@ -5409,7 +5421,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>700</v>
       </c>
@@ -5432,7 +5444,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>701</v>
       </c>
@@ -5455,7 +5467,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>450</v>
       </c>
@@ -5478,7 +5490,7 @@
         <v>43733</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>220</v>
       </c>
@@ -5501,7 +5513,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>108</v>
       </c>
@@ -5524,7 +5536,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>110</v>
       </c>
@@ -5547,7 +5559,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>208</v>
       </c>
@@ -5570,7 +5582,7 @@
         <v>43750</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>648</v>
       </c>
@@ -5593,7 +5605,7 @@
         <v>43750</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>677</v>
       </c>
@@ -5616,7 +5628,7 @@
         <v>43750</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>211</v>
       </c>
@@ -5639,7 +5651,7 @@
         <v>43751</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>421</v>
       </c>
@@ -5662,7 +5674,7 @@
         <v>43751</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>212</v>
       </c>
@@ -5685,7 +5697,7 @@
         <v>43752</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>336</v>
       </c>
@@ -5708,7 +5720,7 @@
         <v>43752</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>215</v>
       </c>
@@ -5731,7 +5743,7 @@
         <v>43753</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>378</v>
       </c>
@@ -5754,7 +5766,7 @@
         <v>43753</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>451</v>
       </c>
@@ -5777,7 +5789,7 @@
         <v>43753</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>973</v>
       </c>
@@ -5800,7 +5812,7 @@
         <v>43753</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>1046</v>
       </c>
@@ -5823,7 +5835,7 @@
         <v>43753</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>692</v>
       </c>
@@ -5846,7 +5858,7 @@
         <v>43754</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>720</v>
       </c>
@@ -5869,7 +5881,7 @@
         <v>43755</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>53</v>
       </c>
@@ -5892,7 +5904,7 @@
         <v>43761</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>121</v>
       </c>
@@ -5915,7 +5927,7 @@
         <v>43761</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>300</v>
       </c>
@@ -5938,7 +5950,7 @@
         <v>43761</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>1025</v>
       </c>
@@ -5961,7 +5973,7 @@
         <v>43761</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>1143</v>
       </c>
@@ -5984,7 +5996,7 @@
         <v>43763</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>72</v>
       </c>
@@ -6007,7 +6019,7 @@
         <v>43768</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>887</v>
       </c>
@@ -6030,7 +6042,7 @@
         <v>43769</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>91</v>
       </c>
@@ -6053,7 +6065,7 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>518</v>
       </c>
@@ -6076,7 +6088,7 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>1221</v>
       </c>
@@ -6099,7 +6111,7 @@
         <v>43773</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>944</v>
       </c>
@@ -6122,7 +6134,7 @@
         <v>43774</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>1029</v>
       </c>
@@ -6145,7 +6157,7 @@
         <v>43774</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>1217</v>
       </c>
@@ -6168,7 +6180,7 @@
         <v>43774</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>455</v>
       </c>
@@ -6191,7 +6203,7 @@
         <v>43775</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>860</v>
       </c>
@@ -6214,7 +6226,7 @@
         <v>43775</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>874</v>
       </c>
@@ -6237,7 +6249,7 @@
         <v>43775</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>1005</v>
       </c>
@@ -6260,7 +6272,7 @@
         <v>43775</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>763</v>
       </c>
@@ -6283,7 +6295,7 @@
         <v>43776</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>921</v>
       </c>
@@ -6306,7 +6318,7 @@
         <v>43777</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>406</v>
       </c>
@@ -6329,7 +6341,7 @@
         <v>43778</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>1090</v>
       </c>
@@ -6352,7 +6364,7 @@
         <v>43778</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>765</v>
       </c>
@@ -6375,7 +6387,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>997</v>
       </c>
@@ -6398,7 +6410,7 @@
         <v>43782</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>1042</v>
       </c>
@@ -6421,7 +6433,7 @@
         <v>43783</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>1161</v>
       </c>
@@ -6444,7 +6456,7 @@
         <v>43783</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>841</v>
       </c>
@@ -6467,7 +6479,7 @@
         <v>43784</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>959</v>
       </c>
@@ -6490,7 +6502,7 @@
         <v>43784</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>1043</v>
       </c>
@@ -6513,7 +6525,7 @@
         <v>43784</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>399</v>
       </c>
@@ -6536,7 +6548,7 @@
         <v>43785</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>684</v>
       </c>
@@ -6559,7 +6571,7 @@
         <v>43785</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>802</v>
       </c>
@@ -6582,7 +6594,7 @@
         <v>43786</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>785</v>
       </c>
@@ -6605,7 +6617,7 @@
         <v>43787</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>996</v>
       </c>
@@ -6628,7 +6640,7 @@
         <v>43788</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>957</v>
       </c>
@@ -6651,7 +6663,7 @@
         <v>43789</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>938</v>
       </c>
@@ -6674,7 +6686,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>1266</v>
       </c>
@@ -6697,7 +6709,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>1281</v>
       </c>
@@ -6720,7 +6732,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>1290</v>
       </c>
@@ -6743,7 +6755,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>1295</v>
       </c>
@@ -6766,7 +6778,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>1313</v>
       </c>
@@ -6789,7 +6801,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>1323</v>
       </c>
@@ -6812,7 +6824,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>1252</v>
       </c>
@@ -6835,7 +6847,7 @@
         <v>43851</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>1309</v>
       </c>
@@ -6858,7 +6870,7 @@
         <v>43851</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>617</v>
       </c>
@@ -6881,7 +6893,7 @@
         <v>43852</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>961</v>
       </c>
@@ -6904,7 +6916,7 @@
         <v>43852</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>1299</v>
       </c>
@@ -6927,7 +6939,7 @@
         <v>43852</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>1304</v>
       </c>
@@ -6950,7 +6962,7 @@
         <v>43852</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>852</v>
       </c>
@@ -6973,7 +6985,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>965</v>
       </c>
@@ -6996,7 +7008,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>1122</v>
       </c>
@@ -7019,7 +7031,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>1207</v>
       </c>
@@ -7042,7 +7054,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>1237</v>
       </c>
@@ -7065,7 +7077,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>1329</v>
       </c>
@@ -7088,7 +7100,7 @@
         <v>43855</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>1331</v>
       </c>
@@ -7111,7 +7123,7 @@
         <v>43855</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>1332</v>
       </c>
@@ -7134,7 +7146,7 @@
         <v>43856</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>463</v>
       </c>
@@ -7157,7 +7169,7 @@
         <v>43857</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>884</v>
       </c>
@@ -7180,7 +7192,7 @@
         <v>43857</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>189</v>
       </c>
@@ -7203,7 +7215,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>897</v>
       </c>
@@ -7226,7 +7238,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>581</v>
       </c>
@@ -7249,7 +7261,7 @@
         <v>43859</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>665</v>
       </c>
@@ -7272,7 +7284,7 @@
         <v>43859</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>1222</v>
       </c>
@@ -7295,7 +7307,7 @@
         <v>43859</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>669</v>
       </c>
@@ -7318,7 +7330,7 @@
         <v>43860</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>1002</v>
       </c>
@@ -7341,7 +7353,7 @@
         <v>43860</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>1160</v>
       </c>
@@ -7364,7 +7376,7 @@
         <v>43860</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>1010</v>
       </c>
@@ -7387,7 +7399,7 @@
         <v>43861</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>821</v>
       </c>
@@ -7410,7 +7422,7 @@
         <v>43864</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>1200</v>
       </c>
@@ -7433,7 +7445,7 @@
         <v>43864</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>1341</v>
       </c>
@@ -7456,7 +7468,7 @@
         <v>43864</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>26</v>
       </c>
@@ -7479,7 +7491,7 @@
         <v>43865</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>27</v>
       </c>
@@ -7502,7 +7514,7 @@
         <v>43865</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>283</v>
       </c>
@@ -7525,7 +7537,7 @@
         <v>43865</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>1030</v>
       </c>
@@ -7548,7 +7560,7 @@
         <v>43865</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>872</v>
       </c>
@@ -7571,7 +7583,7 @@
         <v>43865</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>1022</v>
       </c>
@@ -7594,7 +7606,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>1078</v>
       </c>
@@ -7617,7 +7629,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>930</v>
       </c>
@@ -7640,7 +7652,7 @@
         <v>43867</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>1093</v>
       </c>
@@ -7663,7 +7675,7 @@
         <v>43867</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>15</v>
       </c>
@@ -7686,7 +7698,7 @@
         <v>43868</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>226</v>
       </c>
@@ -7709,7 +7721,7 @@
         <v>43868</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>637</v>
       </c>
@@ -7732,7 +7744,7 @@
         <v>43868</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>1342</v>
       </c>
@@ -7755,7 +7767,7 @@
         <v>43869</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>1343</v>
       </c>
@@ -7778,7 +7790,7 @@
         <v>43869</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>1344</v>
       </c>
@@ -7801,7 +7813,7 @@
         <v>43869</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>209</v>
       </c>
@@ -7824,7 +7836,7 @@
         <v>43871</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>1004</v>
       </c>
@@ -7847,7 +7859,7 @@
         <v>43871</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>1234</v>
       </c>
@@ -7870,7 +7882,7 @@
         <v>43872</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>424</v>
       </c>
@@ -7893,7 +7905,7 @@
         <v>43873</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>567</v>
       </c>
@@ -7916,7 +7928,7 @@
         <v>43873</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>978</v>
       </c>
@@ -7939,7 +7951,7 @@
         <v>43873</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>1208</v>
       </c>
@@ -7962,7 +7974,7 @@
         <v>43874</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>1052</v>
       </c>
@@ -7985,7 +7997,7 @@
         <v>43881</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>1365</v>
       </c>
@@ -8008,7 +8020,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>35</v>
       </c>
@@ -8031,7 +8043,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>1351</v>
       </c>
@@ -8054,7 +8066,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>441</v>
       </c>
@@ -8074,6 +8086,29 @@
         <v>9</v>
       </c>
       <c r="G281" s="19">
+        <v>43894</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A282">
+        <v>475</v>
+      </c>
+      <c r="B282" s="32" t="s">
+        <v>315</v>
+      </c>
+      <c r="C282" t="s">
+        <v>17</v>
+      </c>
+      <c r="D282" t="s">
+        <v>12</v>
+      </c>
+      <c r="E282" t="s">
+        <v>11</v>
+      </c>
+      <c r="F282" t="s">
+        <v>6</v>
+      </c>
+      <c r="G282" s="19">
         <v>43894</v>
       </c>
     </row>
@@ -8125,12 +8160,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -8141,7 +8176,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
@@ -8152,7 +8187,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -8163,7 +8198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -8174,7 +8209,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -8193,92 +8228,92 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>142</v>
       </c>

</xml_diff>